<commit_message>
15/9/ invoice deletion completed
</commit_message>
<xml_diff>
--- a/templatefile/templatefile.xlsx
+++ b/templatefile/templatefile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70e472cbda5f11ee/Desktop/praveen/pdfscrap2/templatefile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Desktop\praveen\new_invoice_automation\templatefile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{C26BE180-0679-41A2-A7EE-50A314EDCA9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{02FF382C-0E71-4F5F-879E-DF7400AEA2A5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722E5ED9-33B0-47AB-9233-1673175EF48E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9225" xr2:uid="{B1655933-1B54-42AE-B284-AB5E17AFD29C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>TRADE PRICE</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>SELLING PRICE(Inc.GST)</t>
+  </si>
+  <si>
+    <t>Filename</t>
   </si>
 </sst>
 </file>
@@ -122,9 +125,14 @@
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -132,12 +140,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -310,37 +313,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -353,6 +358,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -669,147 +680,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE66CF6-CD42-44D4-BF8A-2427CAF9BC75}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" style="3" customWidth="1"/>
-    <col min="5" max="11" width="12.5703125" style="3"/>
-    <col min="12" max="12" width="20.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="3"/>
-    <col min="14" max="14" width="20.42578125" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="12.5703125" style="3"/>
+    <col min="2" max="2" width="10.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="51.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.5703125" style="3"/>
+    <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="3"/>
+    <col min="15" max="15" width="20.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="19" t="s">
+    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="22"/>
+      <c r="I2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="23" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="20"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="22"/>
     </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="21"/>
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="23"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="N4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="K2:N3"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="I2:K3"/>
+    <mergeCell ref="L2:O3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{C94AF447-AC60-414E-A749-FBE65A119875}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>